<commit_message>
feat: update Vendor model to make phone field required, enhance authentication flow, and improve product handling in various components
</commit_message>
<xml_diff>
--- a/prisma/markets.xlsx
+++ b/prisma/markets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Periodic Markets" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="230">
   <si>
     <t xml:space="preserve">Market Name</t>
   </si>
@@ -809,7 +809,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -851,6 +851,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1105,15 +1109,17 @@
   </sheetPr>
   <dimension ref="A1:AB89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F62" activeCellId="0" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="28.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2632,6 +2638,9 @@
       <c r="E61" s="6" t="n">
         <v>45692</v>
       </c>
+      <c r="F61" s="11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7" t="s">
@@ -3121,8 +3130,8 @@
   </sheetPr>
   <dimension ref="A1:AC65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>